<commit_message>
ToF traduction to HAL (in progress)
</commit_message>
<xml_diff>
--- a/Documentation/Devis.xlsx
+++ b/Documentation/Devis.xlsx
@@ -1,23 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T0259172\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lilia\Documents\0_Enseirb_matmeca\3A\S10\Projet industriel\PR324_ST_camera_nocturne\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8142D930-F233-4300-AB3C-D5831DA77BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -191,7 +203,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
   </numFmts>
@@ -235,7 +247,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -245,6 +257,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -352,7 +376,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -370,14 +394,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -658,11 +684,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:A18"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -699,7 +725,7 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="15" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="2">
@@ -720,7 +746,7 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="15" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="2">
@@ -741,7 +767,7 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="2">
@@ -759,10 +785,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="15" t="s">
         <v>42</v>
       </c>
       <c r="C5" s="2">
@@ -780,8 +806,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="4"/>
-      <c r="B6" t="s">
+      <c r="A6" s="14"/>
+      <c r="B6" s="15" t="s">
         <v>44</v>
       </c>
       <c r="C6" s="2">
@@ -799,10 +825,10 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="15" t="s">
         <v>52</v>
       </c>
       <c r="C7" s="2">
@@ -820,7 +846,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B8" t="s">
@@ -834,8 +860,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="11"/>
-      <c r="B9" s="14" t="s">
+      <c r="A9" s="13"/>
+      <c r="B9" s="12" t="s">
         <v>40</v>
       </c>
       <c r="C9" s="2">
@@ -849,7 +875,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B10" t="s">
@@ -863,7 +889,7 @@
       <c r="A11" t="s">
         <v>28</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="15" t="s">
         <v>29</v>
       </c>
       <c r="C11" s="2">
@@ -881,10 +907,10 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="15" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="2">
@@ -902,8 +928,8 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="4"/>
-      <c r="B13" t="s">
+      <c r="A13" s="14"/>
+      <c r="B13" s="16" t="s">
         <v>27</v>
       </c>
       <c r="C13" s="2">
@@ -921,10 +947,10 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="15" t="s">
         <v>49</v>
       </c>
       <c r="C14" s="2">
@@ -942,10 +968,10 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C15" s="2">
@@ -963,8 +989,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="4"/>
-      <c r="B16" t="s">
+      <c r="A16" s="14"/>
+      <c r="B16" s="15" t="s">
         <v>33</v>
       </c>
       <c r="C16" s="2">
@@ -982,8 +1008,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="4"/>
-      <c r="B17" t="s">
+      <c r="A17" s="14"/>
+      <c r="B17" s="15" t="s">
         <v>34</v>
       </c>
       <c r="C17" s="2">
@@ -1001,8 +1027,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="4"/>
-      <c r="B18" t="s">
+      <c r="A18" s="14"/>
+      <c r="B18" s="15" t="s">
         <v>46</v>
       </c>
       <c r="C18" s="2">
@@ -1049,21 +1075,21 @@
     <mergeCell ref="A15:A18"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3" r:id="rId2"/>
-    <hyperlink ref="F4" r:id="rId3" display="https://fr.farnell.com/stmicroelectronics/x-nucleo-cca02m2/carte-ext-microphone-mems-numerique/dp/3262498"/>
-    <hyperlink ref="F12" r:id="rId4" display="https://fr.farnell.com/stmicroelectronics/b-cams-omv/ensemble-de-module-cam-ra-carte/dp/3648877?ost=b-cams-omv"/>
-    <hyperlink ref="F9" r:id="rId5" display="https://fr.rs-online.com/web/p/shields-pour-arduino/2473226"/>
-    <hyperlink ref="F15" r:id="rId6" display="https://fr.farnell.com/multicomp-pro/mp006290/jumper-wire-kit-female-to-female/dp/3617779"/>
-    <hyperlink ref="F17" r:id="rId7" display="https://fr.farnell.com/multicomp-pro/mp006283/jumper-wire-kit-male-to-female/dp/3617771"/>
-    <hyperlink ref="F16" r:id="rId8" display="https://fr.farnell.com/multicomp-pro/mp006282/jumper-wire-kit-male-to-male-100mm/dp/3617770"/>
-    <hyperlink ref="F13" r:id="rId9" display="https://www.gotronic.fr/art-module-camera-ov5640-ada5673-37222.htm"/>
-    <hyperlink ref="F11" r:id="rId10"/>
-    <hyperlink ref="F5" r:id="rId11" display="https://fr.farnell.com/seeed-studio/101020353/carte-capteur-capteur-de-mouvement/dp/3932131"/>
-    <hyperlink ref="F6" r:id="rId12" display="https://fr.farnell.com/on-semiconductor/pir-gevb/carte-evaluation-controleur-detect/dp/2768325"/>
-    <hyperlink ref="F18" r:id="rId13" display="https://fr.farnell.com/seeed-studio/110990028/cavalier-femelle-vers-c-ble-conversion/dp/3932132?st=grove"/>
-    <hyperlink ref="F14" r:id="rId14" display="https://fr.farnell.com/intelligent-led-solutions/ilh-io01-85nl-sc201-wir200/module-metteur-ir-1-chip-ir-850nm/dp/3585881?st=ir%20led"/>
-    <hyperlink ref="F7" r:id="rId15" display="https://fr.farnell.com/seeed-studio/101020132/module-capteur-capteur-de-lumi/dp/3932142"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F4" r:id="rId3" display="https://fr.farnell.com/stmicroelectronics/x-nucleo-cca02m2/carte-ext-microphone-mems-numerique/dp/3262498" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="F12" r:id="rId4" display="https://fr.farnell.com/stmicroelectronics/b-cams-omv/ensemble-de-module-cam-ra-carte/dp/3648877?ost=b-cams-omv" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="F9" r:id="rId5" display="https://fr.rs-online.com/web/p/shields-pour-arduino/2473226" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F15" r:id="rId6" display="https://fr.farnell.com/multicomp-pro/mp006290/jumper-wire-kit-female-to-female/dp/3617779" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="F17" r:id="rId7" display="https://fr.farnell.com/multicomp-pro/mp006283/jumper-wire-kit-male-to-female/dp/3617771" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="F16" r:id="rId8" display="https://fr.farnell.com/multicomp-pro/mp006282/jumper-wire-kit-male-to-male-100mm/dp/3617770" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="F13" r:id="rId9" display="https://www.gotronic.fr/art-module-camera-ov5640-ada5673-37222.htm" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="F11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="F5" r:id="rId11" display="https://fr.farnell.com/seeed-studio/101020353/carte-capteur-capteur-de-mouvement/dp/3932131" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="F6" r:id="rId12" display="https://fr.farnell.com/on-semiconductor/pir-gevb/carte-evaluation-controleur-detect/dp/2768325" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="F18" r:id="rId13" display="https://fr.farnell.com/seeed-studio/110990028/cavalier-femelle-vers-c-ble-conversion/dp/3932132?st=grove" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="F14" r:id="rId14" display="https://fr.farnell.com/intelligent-led-solutions/ilh-io01-85nl-sc201-wir200/module-metteur-ir-1-chip-ir-850nm/dp/3585881?st=ir%20led" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="F7" r:id="rId15" display="https://fr.farnell.com/seeed-studio/101020132/module-capteur-capteur-de-lumi/dp/3932142" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>

</xml_diff>